<commit_message>
updated to latest xlwings version
</commit_message>
<xml_diff>
--- a/reporting/report_template.xlsx
+++ b/reporting/report_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Dev\xlwings-demo\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3250EA4D-AD34-4481-95EF-DEA165BC43B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C7A97F-9FA5-4880-954E-652142A3047E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="Table1">Sheet1!#REF!</definedName>
-    <definedName name="Table2">Sheet1!$A$13</definedName>
+    <definedName name="Table2">Sheet1!$A$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,14 +36,46 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Felix Zumstein</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{7A415746-855B-48BF-83A1-77C791597C5A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>&lt;frame&gt;</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{9747C3F0-9699-4ABB-A76C-88231ECDC9D1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>&lt;frame&gt;</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
-  <si>
-    <t>{{ logo }}</t>
-  </si>
-  <si>
-    <t>The performance was {{ perf }}%.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>{{ perf_data }}</t>
   </si>
@@ -51,20 +83,26 @@
     <t>{{ fig }}</t>
   </si>
   <si>
-    <t>&lt;frame&gt;</t>
-  </si>
-  <si>
     <t>c1</t>
   </si>
   <si>
     <t>r1</t>
+  </si>
+  <si>
+    <t>{{ logo | scale(0.8) }}</t>
+  </si>
+  <si>
+    <t>The performance was {{ perf | format(".1%") }}.</t>
+  </si>
+  <si>
+    <t>r2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -99,6 +137,19 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -151,11 +202,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -166,7 +218,10 @@
     <cellStyle name="Normal 2 3" xfId="4" xr:uid="{EC3587A3-A887-9449-9DA5-2BBB27048313}"/>
     <cellStyle name="Per cent 2" xfId="5" xr:uid="{7CEF30C3-0624-F844-9DB8-D27AFAD27A86}"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -222,7 +277,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$10</c:f>
+              <c:f>Sheet1!$B$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -271,7 +326,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$11</c:f>
+              <c:f>Sheet1!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -282,7 +337,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$11</c:f>
+              <c:f>Sheet1!$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -295,6 +350,84 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2466-4E63-A778-31C1832577CC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>r2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>c1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BE47-4CBD-9AE8-56B6E3E0868B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1038,13 +1171,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>33338</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>757237</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>14288</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1106,13 +1239,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>35728</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>747712</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>119063</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1142,14 +1275,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1E3CED49-96F5-4C81-B040-296DF187A41B}" name="Table6" displayName="Table6" ref="A10:B11" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A10:B11" xr:uid="{1D0B1C0C-B0E7-4A60-9DA5-6A70A0E081BC}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1E3CED49-96F5-4C81-B040-296DF187A41B}" name="Table6" displayName="Table6" ref="A9:C10" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A9:C10" xr:uid="{1D0B1C0C-B0E7-4A60-9DA5-6A70A0E081BC}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="2">
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{6E4AEC87-F834-4B9C-A4F7-389567F50E21}" name="{{ perf_data }}" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{95601B00-4023-4D02-AD87-6F56F0E083C6}" name="r1" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{C6752B97-DA8F-4385-BD7E-07C84E8EFE23}" name="r2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1451,11 +1586,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C37306-6492-634D-B59F-CECAA69C603C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C37306-6492-634D-B59F-CECAA69C603C}">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1466,48 +1601,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A1" s="2"/>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A8" s="1" t="s">
-        <v>1</v>
+      <c r="C9" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="1">
+      <c r="B10" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>